<commit_message>
fix typos and grammers
</commit_message>
<xml_diff>
--- a/_cv_data/cv_entries.xlsx
+++ b/_cv_data/cv_entries.xlsx
@@ -100,7 +100,7 @@
     <t>CarOpp, New York, USA</t>
   </si>
   <si>
-    <t xml:space="preserve">Promoted to join new team developing a rental private cars that allow users to store data and pay rental fees using ruby on rails. Worked as a member of team that had established in California. Developed new features according to product roadmap and requirements. </t>
+    <t xml:space="preserve">Leading a team of developers to develop and maintain a backend/frontend stack for car rental management application. </t>
   </si>
   <si>
     <t>Software EngineerII</t>
@@ -109,7 +109,7 @@
     <t>Cognizant, New York, USA</t>
   </si>
   <si>
-    <t xml:space="preserve">Collaborated with designers to create clean interfaces and simple, intuitive interactions and experiences. Designed embeded systems software by applying key principles of computer science, engineering, and mathematical analysis. Oversaw software system installation and collaborated on implementation of new features. Delivered software solutions consistent with the product roadmap and release plan milestones through Agile environment. Document continuously for easy reference and to keep entire team up-to date on changes. Analyze software usability and performance to improve functionality. Collaborated with the quality engineers to sync unit tests with integration tests before deploying. </t>
+    <t>I assisted in developing new software to provide more productive ways of interacting with the model. Additionally, I was responsible for analyzing software usability and performance to improve functionality.  I delivered software solutions consistent with the product roadmap and release plan milestones through the agile environment. I worked with the quality engineers to sync unit tests with integration tests before deploying. I was involved in writing an SQL query for data extraction and management (MySQL and PostgreSQL). I managed an elastic search query for a recommendation based on specific criteria. Too, I was qualified to draft 100+ instructional documents.</t>
   </si>
   <si>
     <t>2009</t>
@@ -124,7 +124,7 @@
     <t>Octomedical</t>
   </si>
   <si>
-    <t xml:space="preserve">Responsible for designing equipments for Pharma industry </t>
+    <t xml:space="preserve">Responsible for designing equipment for the Pharma industry </t>
   </si>
   <si>
     <t>Maintenance Engineer</t>

</xml_diff>